<commit_message>
final comments and tests before merging
This branch should be merged to continue work on #220 and other related
issues of Gabriel Happle.
Archetype properties are exemplary. No research has been done so far.
All AC cooled buildings ('type_cs = T3') are mechanically ventilated. So
are also all industrial and special use buildings (server, coolroom,
etc).
None of the buildings have economizers or night flushing.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/Archetypes/Archetypes_properties.xlsx
+++ b/cea/databases/CH/Archetypes/Archetypes_properties.xlsx
@@ -867,18 +867,6 @@
     <t>T5</t>
   </si>
   <si>
-    <t>HEAT_RECOVERY</t>
-  </si>
-  <si>
-    <t>WINDOW_VENTILATION</t>
-  </si>
-  <si>
-    <t>MECHANICAL_VENTILATION</t>
-  </si>
-  <si>
-    <t>NIGHT_FLUSHING</t>
-  </si>
-  <si>
     <t>ECONOMIZER</t>
   </si>
   <si>
@@ -901,6 +889,18 @@
   </si>
   <si>
     <t>WVE0</t>
+  </si>
+  <si>
+    <t>MECH_VENT</t>
+  </si>
+  <si>
+    <t>WIN_VENT</t>
+  </si>
+  <si>
+    <t>HEAT_REC</t>
+  </si>
+  <si>
+    <t>NIGHT_FLSH</t>
   </si>
 </sst>
 </file>
@@ -8721,7 +8721,7 @@
   <dimension ref="A1:L181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I181" sqref="I181"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8763,19 +8763,19 @@
         <v>9</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="J1" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>280</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -8801,19 +8801,19 @@
         <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -8839,19 +8839,19 @@
         <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -8877,19 +8877,19 @@
         <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -8915,19 +8915,19 @@
         <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -8953,19 +8953,19 @@
         <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -8991,19 +8991,19 @@
         <v>17</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -9029,19 +9029,19 @@
         <v>18</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -9067,19 +9067,19 @@
         <v>18</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -9105,19 +9105,19 @@
         <v>18</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -9143,19 +9143,19 @@
         <v>18</v>
       </c>
       <c r="H11" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -9181,19 +9181,19 @@
         <v>20</v>
       </c>
       <c r="H12" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -9219,19 +9219,19 @@
         <v>17</v>
       </c>
       <c r="H13" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -9257,19 +9257,19 @@
         <v>18</v>
       </c>
       <c r="H14" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -9295,19 +9295,19 @@
         <v>18</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -9333,19 +9333,19 @@
         <v>18</v>
       </c>
       <c r="H16" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -9371,19 +9371,19 @@
         <v>18</v>
       </c>
       <c r="H17" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -9409,19 +9409,19 @@
         <v>20</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -9447,19 +9447,19 @@
         <v>17</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -9485,19 +9485,19 @@
         <v>18</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -9523,19 +9523,19 @@
         <v>18</v>
       </c>
       <c r="H21" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -9561,19 +9561,19 @@
         <v>18</v>
       </c>
       <c r="H22" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -9599,19 +9599,19 @@
         <v>18</v>
       </c>
       <c r="H23" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -9637,19 +9637,19 @@
         <v>20</v>
       </c>
       <c r="H24" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -9675,19 +9675,19 @@
         <v>17</v>
       </c>
       <c r="H25" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -9713,19 +9713,19 @@
         <v>18</v>
       </c>
       <c r="H26" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -9751,19 +9751,19 @@
         <v>18</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -9789,19 +9789,19 @@
         <v>18</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -9827,19 +9827,19 @@
         <v>18</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -9865,19 +9865,19 @@
         <v>20</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -9903,19 +9903,19 @@
         <v>17</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -9941,19 +9941,19 @@
         <v>18</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -9979,19 +9979,19 @@
         <v>18</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -10017,19 +10017,19 @@
         <v>18</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -10055,19 +10055,19 @@
         <v>18</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -10093,19 +10093,19 @@
         <v>20</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -10131,19 +10131,19 @@
         <v>17</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -10169,19 +10169,19 @@
         <v>18</v>
       </c>
       <c r="H38" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L38" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -10207,19 +10207,19 @@
         <v>18</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -10245,19 +10245,19 @@
         <v>18</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -10283,19 +10283,19 @@
         <v>18</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -10321,19 +10321,19 @@
         <v>20</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -10359,19 +10359,19 @@
         <v>17</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -10397,19 +10397,19 @@
         <v>18</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -10435,19 +10435,19 @@
         <v>18</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -10473,19 +10473,19 @@
         <v>18</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -10511,19 +10511,19 @@
         <v>18</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -10549,19 +10549,19 @@
         <v>20</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -10587,19 +10587,19 @@
         <v>17</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -10625,19 +10625,19 @@
         <v>18</v>
       </c>
       <c r="H50" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L50" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -10663,19 +10663,19 @@
         <v>18</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -10701,19 +10701,19 @@
         <v>18</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -10739,19 +10739,19 @@
         <v>18</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -10777,19 +10777,19 @@
         <v>20</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -10815,19 +10815,19 @@
         <v>17</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -10853,19 +10853,19 @@
         <v>18</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -10891,19 +10891,19 @@
         <v>18</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -10929,19 +10929,19 @@
         <v>18</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -10967,19 +10967,19 @@
         <v>18</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -11005,19 +11005,19 @@
         <v>20</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -11043,19 +11043,19 @@
         <v>17</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -11081,19 +11081,19 @@
         <v>18</v>
       </c>
       <c r="H62" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L62" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L62" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -11119,19 +11119,19 @@
         <v>18</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -11157,19 +11157,19 @@
         <v>18</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -11195,19 +11195,19 @@
         <v>18</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -11233,19 +11233,19 @@
         <v>20</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -11271,19 +11271,19 @@
         <v>17</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -11309,19 +11309,19 @@
         <v>18</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -11347,19 +11347,19 @@
         <v>18</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -11385,19 +11385,19 @@
         <v>18</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -11423,19 +11423,19 @@
         <v>18</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -11461,19 +11461,19 @@
         <v>20</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -11499,19 +11499,19 @@
         <v>17</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -11537,19 +11537,19 @@
         <v>18</v>
       </c>
       <c r="H74" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L74" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -11575,19 +11575,19 @@
         <v>18</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K75" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -11613,19 +11613,19 @@
         <v>18</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -11651,19 +11651,19 @@
         <v>18</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -11689,19 +11689,19 @@
         <v>20</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -11727,19 +11727,19 @@
         <v>17</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -11765,19 +11765,19 @@
         <v>18</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K80" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -11803,19 +11803,19 @@
         <v>18</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -11841,19 +11841,19 @@
         <v>18</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -11879,19 +11879,19 @@
         <v>18</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -11917,19 +11917,19 @@
         <v>20</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K84" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -11955,19 +11955,19 @@
         <v>17</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -11993,19 +11993,19 @@
         <v>18</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -12031,19 +12031,19 @@
         <v>18</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -12069,19 +12069,19 @@
         <v>18</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -12107,19 +12107,19 @@
         <v>18</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -12145,19 +12145,19 @@
         <v>20</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -12183,19 +12183,19 @@
         <v>17</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -12221,19 +12221,19 @@
         <v>18</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -12259,19 +12259,19 @@
         <v>18</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -12297,19 +12297,19 @@
         <v>18</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K94" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L94" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -12335,19 +12335,19 @@
         <v>18</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K95" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L95" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -12373,19 +12373,19 @@
         <v>20</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K96" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -12411,19 +12411,19 @@
         <v>17</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -12449,19 +12449,19 @@
         <v>18</v>
       </c>
       <c r="H98" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L98" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I98" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J98" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K98" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L98" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -12487,19 +12487,19 @@
         <v>18</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K99" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -12525,19 +12525,19 @@
         <v>18</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K100" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L100" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -12563,19 +12563,19 @@
         <v>18</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L101" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -12601,19 +12601,19 @@
         <v>20</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K102" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L102" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -12639,19 +12639,19 @@
         <v>17</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K103" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L103" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -12677,19 +12677,19 @@
         <v>18</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L104" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
@@ -12715,19 +12715,19 @@
         <v>18</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K105" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L105" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -12753,19 +12753,19 @@
         <v>18</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L106" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -12791,19 +12791,19 @@
         <v>18</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L107" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -12829,19 +12829,19 @@
         <v>20</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K108" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L108" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -12867,19 +12867,19 @@
         <v>17</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L109" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -12905,19 +12905,19 @@
         <v>18</v>
       </c>
       <c r="H110" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L110" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J110" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K110" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L110" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
@@ -12943,19 +12943,19 @@
         <v>18</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K111" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L111" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
@@ -12981,19 +12981,19 @@
         <v>18</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K112" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L112" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -13019,19 +13019,19 @@
         <v>18</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K113" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L113" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -13057,19 +13057,19 @@
         <v>20</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L114" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
@@ -13095,19 +13095,19 @@
         <v>17</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J115" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L115" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
@@ -13133,19 +13133,19 @@
         <v>18</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K116" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L116" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
@@ -13171,19 +13171,19 @@
         <v>18</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J117" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K117" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L117" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
@@ -13209,19 +13209,19 @@
         <v>18</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J118" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K118" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
@@ -13247,19 +13247,19 @@
         <v>18</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K119" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L119" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
@@ -13285,19 +13285,19 @@
         <v>20</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J120" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L120" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
@@ -13323,19 +13323,19 @@
         <v>17</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K121" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L121" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
@@ -13361,19 +13361,19 @@
         <v>18</v>
       </c>
       <c r="H122" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K122" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L122" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J122" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K122" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L122" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
@@ -13399,19 +13399,19 @@
         <v>18</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K123" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L123" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
@@ -13437,19 +13437,19 @@
         <v>18</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J124" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L124" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
@@ -13475,19 +13475,19 @@
         <v>18</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J125" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K125" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L125" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
@@ -13513,19 +13513,19 @@
         <v>20</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J126" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K126" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L126" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
@@ -13551,19 +13551,19 @@
         <v>17</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K127" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L127" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
@@ -13589,19 +13589,19 @@
         <v>18</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J128" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K128" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L128" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
@@ -13627,19 +13627,19 @@
         <v>18</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J129" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K129" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L129" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -13665,19 +13665,19 @@
         <v>18</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J130" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K130" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L130" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
@@ -13703,19 +13703,19 @@
         <v>18</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J131" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K131" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L131" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
@@ -13741,19 +13741,19 @@
         <v>20</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K132" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L132" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
@@ -13779,19 +13779,19 @@
         <v>17</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K133" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L133" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -13817,19 +13817,19 @@
         <v>18</v>
       </c>
       <c r="H134" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L134" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J134" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K134" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L134" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
@@ -13855,19 +13855,19 @@
         <v>18</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J135" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L135" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -13893,19 +13893,19 @@
         <v>18</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J136" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K136" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L136" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
@@ -13931,19 +13931,19 @@
         <v>18</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J137" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K137" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L137" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
@@ -13969,19 +13969,19 @@
         <v>20</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K138" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L138" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
@@ -14007,19 +14007,19 @@
         <v>17</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I139" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J139" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K139" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L139" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
@@ -14045,19 +14045,19 @@
         <v>18</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J140" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L140" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
@@ -14083,19 +14083,19 @@
         <v>18</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I141" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J141" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K141" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L141" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
@@ -14121,19 +14121,19 @@
         <v>18</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I142" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J142" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K142" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L142" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
@@ -14159,19 +14159,19 @@
         <v>18</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K143" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L143" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
@@ -14197,19 +14197,19 @@
         <v>20</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I144" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J144" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K144" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L144" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
@@ -14235,19 +14235,19 @@
         <v>17</v>
       </c>
       <c r="H145" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K145" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L145" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
@@ -14273,19 +14273,19 @@
         <v>18</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I146" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J146" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K146" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L146" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
@@ -14311,19 +14311,19 @@
         <v>18</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J147" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K147" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L147" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
@@ -14349,19 +14349,19 @@
         <v>18</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J148" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K148" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L148" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
@@ -14387,19 +14387,19 @@
         <v>18</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I149" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J149" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K149" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L149" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
@@ -14425,19 +14425,19 @@
         <v>20</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J150" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K150" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L150" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
@@ -14463,19 +14463,19 @@
         <v>17</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J151" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K151" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L151" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
@@ -14501,19 +14501,19 @@
         <v>18</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J152" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K152" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L152" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
@@ -14539,19 +14539,19 @@
         <v>18</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J153" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K153" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L153" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
@@ -14577,19 +14577,19 @@
         <v>18</v>
       </c>
       <c r="H154" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I154" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J154" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K154" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L154" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
@@ -14615,19 +14615,19 @@
         <v>18</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J155" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K155" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L155" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
@@ -14653,19 +14653,19 @@
         <v>20</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J156" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K156" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L156" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
@@ -14691,19 +14691,19 @@
         <v>17</v>
       </c>
       <c r="H157" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J157" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K157" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L157" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
@@ -14729,19 +14729,19 @@
         <v>19</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J158" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K158" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L158" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
@@ -14767,19 +14767,19 @@
         <v>19</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J159" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K159" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L159" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
@@ -14805,19 +14805,19 @@
         <v>19</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I160" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J160" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K160" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L160" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
@@ -14843,19 +14843,19 @@
         <v>19</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I161" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J161" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K161" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L161" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
@@ -14881,19 +14881,19 @@
         <v>19</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I162" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J162" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K162" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L162" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
@@ -14919,19 +14919,19 @@
         <v>19</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J163" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K163" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L163" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
@@ -14957,19 +14957,19 @@
         <v>19</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I164" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J164" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K164" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L164" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
@@ -14995,19 +14995,19 @@
         <v>19</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I165" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J165" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K165" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L165" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.25">
@@ -15033,19 +15033,19 @@
         <v>19</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I166" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J166" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K166" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L166" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
@@ -15071,19 +15071,19 @@
         <v>19</v>
       </c>
       <c r="H167" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I167" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J167" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K167" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L167" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
@@ -15109,19 +15109,19 @@
         <v>19</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J168" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K168" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L168" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.25">
@@ -15147,19 +15147,19 @@
         <v>19</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I169" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J169" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K169" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L169" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
@@ -15185,19 +15185,19 @@
         <v>18</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I170" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J170" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K170" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L170" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
@@ -15223,19 +15223,19 @@
         <v>18</v>
       </c>
       <c r="H171" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I171" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J171" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K171" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L171" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.25">
@@ -15261,19 +15261,19 @@
         <v>18</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J172" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K172" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L172" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.25">
@@ -15299,19 +15299,19 @@
         <v>18</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I173" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J173" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K173" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L173" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
@@ -15337,19 +15337,19 @@
         <v>20</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J174" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K174" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L174" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
@@ -15375,19 +15375,19 @@
         <v>17</v>
       </c>
       <c r="H175" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J175" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K175" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L175" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
@@ -15413,19 +15413,19 @@
         <v>18</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J176" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K176" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L176" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.25">
@@ -15451,19 +15451,19 @@
         <v>18</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I177" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J177" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K177" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L177" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.25">
@@ -15489,19 +15489,19 @@
         <v>18</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J178" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K178" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L178" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.25">
@@ -15527,19 +15527,19 @@
         <v>18</v>
       </c>
       <c r="H179" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J179" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K179" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L179" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.25">
@@ -15565,19 +15565,19 @@
         <v>20</v>
       </c>
       <c r="H180" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I180" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J180" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K180" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L180" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.25">
@@ -15603,19 +15603,19 @@
         <v>17</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J181" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K181" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L181" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new attempt on ventilation system properties
according to discussion with @JIMENOFONSECA
</commit_message>
<xml_diff>
--- a/cea/databases/CH/Archetypes/Archetypes_properties.xlsx
+++ b/cea/databases/CH/Archetypes/Archetypes_properties.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5181" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4457" uniqueCount="281">
   <si>
     <t>Code</t>
   </si>
@@ -867,40 +867,7 @@
     <t>T5</t>
   </si>
   <si>
-    <t>ECONOMIZER</t>
-  </si>
-  <si>
-    <t>MVE0</t>
-  </si>
-  <si>
-    <t>WVE1</t>
-  </si>
-  <si>
-    <t>NFL0</t>
-  </si>
-  <si>
-    <t>HRE0</t>
-  </si>
-  <si>
-    <t>ECO0</t>
-  </si>
-  <si>
-    <t>MVE1</t>
-  </si>
-  <si>
-    <t>WVE0</t>
-  </si>
-  <si>
-    <t>MECH_VENT</t>
-  </si>
-  <si>
-    <t>WIN_VENT</t>
-  </si>
-  <si>
-    <t>HEAT_REC</t>
-  </si>
-  <si>
-    <t>NIGHT_FLSH</t>
+    <t>type_vent</t>
   </si>
 </sst>
 </file>
@@ -8718,10 +8685,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L181"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8732,15 +8699,11 @@
     <col min="4" max="5" width="9.140625" style="4"/>
     <col min="6" max="6" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="11.28515625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -8763,22 +8726,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="L1" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -8801,22 +8752,10 @@
         <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>30</v>
       </c>
@@ -8839,22 +8778,10 @@
         <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
@@ -8877,22 +8804,10 @@
         <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>32</v>
       </c>
@@ -8915,22 +8830,10 @@
         <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
@@ -8953,22 +8856,10 @@
         <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>34</v>
       </c>
@@ -8991,22 +8882,10 @@
         <v>17</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>35</v>
       </c>
@@ -9029,22 +8908,10 @@
         <v>18</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>36</v>
       </c>
@@ -9067,22 +8934,10 @@
         <v>18</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>37</v>
       </c>
@@ -9105,22 +8960,10 @@
         <v>18</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>38</v>
       </c>
@@ -9143,22 +8986,10 @@
         <v>18</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>39</v>
       </c>
@@ -9181,22 +9012,10 @@
         <v>20</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>40</v>
       </c>
@@ -9219,22 +9038,10 @@
         <v>17</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -9257,22 +9064,10 @@
         <v>18</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>54</v>
       </c>
@@ -9295,22 +9090,10 @@
         <v>18</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>55</v>
       </c>
@@ -9333,22 +9116,10 @@
         <v>18</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>56</v>
       </c>
@@ -9371,22 +9142,10 @@
         <v>18</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>57</v>
       </c>
@@ -9409,22 +9168,10 @@
         <v>20</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>58</v>
       </c>
@@ -9447,22 +9194,10 @@
         <v>17</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>59</v>
       </c>
@@ -9485,22 +9220,10 @@
         <v>18</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>60</v>
       </c>
@@ -9523,22 +9246,10 @@
         <v>18</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>61</v>
       </c>
@@ -9561,22 +9272,10 @@
         <v>18</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>62</v>
       </c>
@@ -9599,22 +9298,10 @@
         <v>18</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>63</v>
       </c>
@@ -9637,22 +9324,10 @@
         <v>20</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>64</v>
       </c>
@@ -9675,22 +9350,10 @@
         <v>17</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>41</v>
       </c>
@@ -9713,22 +9376,10 @@
         <v>18</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
@@ -9751,22 +9402,10 @@
         <v>18</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
@@ -9789,22 +9428,10 @@
         <v>18</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -9827,22 +9454,10 @@
         <v>18</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -9865,22 +9480,10 @@
         <v>20</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>46</v>
       </c>
@@ -9903,22 +9506,10 @@
         <v>17</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>47</v>
       </c>
@@ -9941,22 +9532,10 @@
         <v>18</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>48</v>
       </c>
@@ -9979,22 +9558,10 @@
         <v>18</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>49</v>
       </c>
@@ -10017,22 +9584,10 @@
         <v>18</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>50</v>
       </c>
@@ -10055,22 +9610,10 @@
         <v>18</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>51</v>
       </c>
@@ -10093,22 +9636,10 @@
         <v>20</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>52</v>
       </c>
@@ -10131,22 +9662,10 @@
         <v>17</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>65</v>
       </c>
@@ -10169,22 +9688,10 @@
         <v>18</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>66</v>
       </c>
@@ -10207,22 +9714,10 @@
         <v>18</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>67</v>
       </c>
@@ -10245,22 +9740,10 @@
         <v>18</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>68</v>
       </c>
@@ -10283,22 +9766,10 @@
         <v>18</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>69</v>
       </c>
@@ -10321,22 +9792,10 @@
         <v>20</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>70</v>
       </c>
@@ -10359,22 +9818,10 @@
         <v>17</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>71</v>
       </c>
@@ -10397,22 +9844,10 @@
         <v>18</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>72</v>
       </c>
@@ -10435,22 +9870,10 @@
         <v>18</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>73</v>
       </c>
@@ -10473,22 +9896,10 @@
         <v>18</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>74</v>
       </c>
@@ -10511,22 +9922,10 @@
         <v>18</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>75</v>
       </c>
@@ -10549,22 +9948,10 @@
         <v>20</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L48" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>76</v>
       </c>
@@ -10587,22 +9974,10 @@
         <v>17</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>77</v>
       </c>
@@ -10625,22 +10000,10 @@
         <v>18</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>78</v>
       </c>
@@ -10663,22 +10026,10 @@
         <v>18</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>79</v>
       </c>
@@ -10701,22 +10052,10 @@
         <v>18</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>80</v>
       </c>
@@ -10739,22 +10078,10 @@
         <v>18</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>81</v>
       </c>
@@ -10777,22 +10104,10 @@
         <v>20</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>82</v>
       </c>
@@ -10815,22 +10130,10 @@
         <v>17</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>83</v>
       </c>
@@ -10853,22 +10156,10 @@
         <v>18</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L56" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>84</v>
       </c>
@@ -10891,22 +10182,10 @@
         <v>18</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>85</v>
       </c>
@@ -10929,22 +10208,10 @@
         <v>18</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K58" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L58" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>86</v>
       </c>
@@ -10967,22 +10234,10 @@
         <v>18</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K59" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L59" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>87</v>
       </c>
@@ -11005,22 +10260,10 @@
         <v>20</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K60" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L60" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>88</v>
       </c>
@@ -11043,22 +10286,10 @@
         <v>17</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K61" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L61" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>257</v>
       </c>
@@ -11081,22 +10312,10 @@
         <v>18</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L62" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>258</v>
       </c>
@@ -11119,22 +10338,10 @@
         <v>18</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L63" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>259</v>
       </c>
@@ -11157,22 +10364,10 @@
         <v>18</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L64" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>260</v>
       </c>
@@ -11195,22 +10390,10 @@
         <v>18</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L65" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>261</v>
       </c>
@@ -11233,22 +10416,10 @@
         <v>20</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K66" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L66" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>262</v>
       </c>
@@ -11271,22 +10442,10 @@
         <v>17</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L67" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>263</v>
       </c>
@@ -11309,22 +10468,10 @@
         <v>18</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L68" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>264</v>
       </c>
@@ -11347,22 +10494,10 @@
         <v>18</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L69" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>265</v>
       </c>
@@ -11385,22 +10520,10 @@
         <v>18</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I70" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L70" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>266</v>
       </c>
@@ -11423,22 +10546,10 @@
         <v>18</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L71" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>267</v>
       </c>
@@ -11461,22 +10572,10 @@
         <v>20</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>268</v>
       </c>
@@ -11499,22 +10598,10 @@
         <v>17</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>101</v>
       </c>
@@ -11537,22 +10624,10 @@
         <v>18</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>102</v>
       </c>
@@ -11575,22 +10650,10 @@
         <v>18</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L75" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>103</v>
       </c>
@@ -11613,22 +10676,10 @@
         <v>18</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K76" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L76" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>104</v>
       </c>
@@ -11651,22 +10702,10 @@
         <v>18</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K77" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L77" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>105</v>
       </c>
@@ -11689,22 +10728,10 @@
         <v>20</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J78" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K78" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L78" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>106</v>
       </c>
@@ -11727,22 +10754,10 @@
         <v>17</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J79" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K79" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L79" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>107</v>
       </c>
@@ -11765,22 +10780,10 @@
         <v>18</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J80" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L80" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>108</v>
       </c>
@@ -11803,22 +10806,10 @@
         <v>18</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L81" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>109</v>
       </c>
@@ -11841,22 +10832,10 @@
         <v>18</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I82" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K82" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L82" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>110</v>
       </c>
@@ -11879,22 +10858,10 @@
         <v>18</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J83" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K83" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L83" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>111</v>
       </c>
@@ -11917,22 +10884,10 @@
         <v>20</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J84" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K84" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L84" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>112</v>
       </c>
@@ -11955,22 +10910,10 @@
         <v>17</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J85" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K85" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L85" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>113</v>
       </c>
@@ -11993,22 +10936,10 @@
         <v>18</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J86" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K86" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L86" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>114</v>
       </c>
@@ -12031,22 +10962,10 @@
         <v>18</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K87" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L87" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>115</v>
       </c>
@@ -12069,22 +10988,10 @@
         <v>18</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K88" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L88" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>116</v>
       </c>
@@ -12107,22 +11014,10 @@
         <v>18</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L89" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>117</v>
       </c>
@@ -12145,22 +11040,10 @@
         <v>20</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I90" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J90" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K90" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L90" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>118</v>
       </c>
@@ -12183,22 +11066,10 @@
         <v>17</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I91" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J91" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K91" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L91" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>119</v>
       </c>
@@ -12221,22 +11092,10 @@
         <v>18</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I92" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J92" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K92" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L92" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>120</v>
       </c>
@@ -12259,22 +11118,10 @@
         <v>18</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I93" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J93" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K93" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L93" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>121</v>
       </c>
@@ -12297,22 +11144,10 @@
         <v>18</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I94" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J94" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K94" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L94" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>122</v>
       </c>
@@ -12335,22 +11170,10 @@
         <v>18</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J95" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K95" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L95" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>123</v>
       </c>
@@ -12373,22 +11196,10 @@
         <v>20</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I96" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J96" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K96" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L96" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>124</v>
       </c>
@@ -12411,22 +11222,10 @@
         <v>17</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I97" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J97" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K97" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L97" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>125</v>
       </c>
@@ -12449,22 +11248,10 @@
         <v>18</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I98" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J98" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K98" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L98" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>126</v>
       </c>
@@ -12487,22 +11274,10 @@
         <v>18</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I99" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J99" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K99" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L99" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>127</v>
       </c>
@@ -12525,22 +11300,10 @@
         <v>18</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I100" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K100" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L100" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>128</v>
       </c>
@@ -12563,22 +11326,10 @@
         <v>18</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I101" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K101" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L101" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>129</v>
       </c>
@@ -12601,22 +11352,10 @@
         <v>20</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I102" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J102" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K102" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L102" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>130</v>
       </c>
@@ -12639,22 +11378,10 @@
         <v>17</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I103" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L103" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>131</v>
       </c>
@@ -12677,22 +11404,10 @@
         <v>18</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J104" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K104" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L104" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>132</v>
       </c>
@@ -12715,22 +11430,10 @@
         <v>18</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J105" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K105" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L105" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>133</v>
       </c>
@@ -12753,22 +11456,10 @@
         <v>18</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K106" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L106" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>134</v>
       </c>
@@ -12791,22 +11482,10 @@
         <v>18</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I107" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J107" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K107" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L107" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>135</v>
       </c>
@@ -12829,22 +11508,10 @@
         <v>20</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J108" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K108" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L108" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>136</v>
       </c>
@@ -12867,22 +11534,10 @@
         <v>17</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I109" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J109" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K109" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L109" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>137</v>
       </c>
@@ -12905,22 +11560,10 @@
         <v>18</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J110" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K110" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L110" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>138</v>
       </c>
@@ -12943,22 +11586,10 @@
         <v>18</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I111" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J111" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K111" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L111" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>139</v>
       </c>
@@ -12981,22 +11612,10 @@
         <v>18</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J112" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K112" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L112" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>140</v>
       </c>
@@ -13019,22 +11638,10 @@
         <v>18</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J113" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K113" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L113" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>141</v>
       </c>
@@ -13057,22 +11664,10 @@
         <v>20</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I114" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J114" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K114" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L114" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>142</v>
       </c>
@@ -13095,22 +11690,10 @@
         <v>17</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I115" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J115" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K115" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L115" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>143</v>
       </c>
@@ -13133,22 +11716,10 @@
         <v>18</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J116" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K116" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L116" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>144</v>
       </c>
@@ -13171,22 +11742,10 @@
         <v>18</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I117" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J117" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K117" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L117" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>145</v>
       </c>
@@ -13209,22 +11768,10 @@
         <v>18</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J118" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K118" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L118" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>146</v>
       </c>
@@ -13247,22 +11794,10 @@
         <v>18</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J119" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K119" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L119" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>147</v>
       </c>
@@ -13285,22 +11820,10 @@
         <v>20</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I120" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K120" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L120" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
         <v>148</v>
       </c>
@@ -13323,22 +11846,10 @@
         <v>17</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I121" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J121" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K121" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L121" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
         <v>149</v>
       </c>
@@ -13361,22 +11872,10 @@
         <v>18</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J122" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K122" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L122" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>150</v>
       </c>
@@ -13399,22 +11898,10 @@
         <v>18</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I123" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J123" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K123" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L123" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>151</v>
       </c>
@@ -13437,22 +11924,10 @@
         <v>18</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I124" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J124" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K124" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L124" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>152</v>
       </c>
@@ -13475,22 +11950,10 @@
         <v>18</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I125" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J125" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K125" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L125" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
         <v>153</v>
       </c>
@@ -13513,22 +11976,10 @@
         <v>20</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I126" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J126" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K126" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L126" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
         <v>154</v>
       </c>
@@ -13551,22 +12002,10 @@
         <v>17</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I127" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J127" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K127" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L127" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>155</v>
       </c>
@@ -13589,22 +12028,10 @@
         <v>18</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I128" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J128" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K128" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L128" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>156</v>
       </c>
@@ -13627,22 +12054,10 @@
         <v>18</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I129" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J129" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K129" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L129" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>157</v>
       </c>
@@ -13665,22 +12080,10 @@
         <v>18</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J130" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K130" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L130" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>158</v>
       </c>
@@ -13703,22 +12106,10 @@
         <v>18</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I131" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J131" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K131" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L131" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>159</v>
       </c>
@@ -13741,22 +12132,10 @@
         <v>20</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I132" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J132" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K132" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L132" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>160</v>
       </c>
@@ -13779,22 +12158,10 @@
         <v>17</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I133" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J133" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K133" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L133" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>161</v>
       </c>
@@ -13817,22 +12184,10 @@
         <v>18</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J134" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K134" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L134" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
         <v>162</v>
       </c>
@@ -13855,22 +12210,10 @@
         <v>18</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J135" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K135" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L135" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>163</v>
       </c>
@@ -13893,22 +12236,10 @@
         <v>18</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I136" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J136" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K136" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L136" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
         <v>164</v>
       </c>
@@ -13931,22 +12262,10 @@
         <v>18</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I137" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J137" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K137" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L137" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
         <v>165</v>
       </c>
@@ -13969,22 +12288,10 @@
         <v>20</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I138" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J138" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K138" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L138" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>166</v>
       </c>
@@ -14007,22 +12314,10 @@
         <v>17</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I139" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J139" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K139" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L139" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
         <v>167</v>
       </c>
@@ -14045,22 +12340,10 @@
         <v>18</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I140" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J140" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K140" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L140" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>168</v>
       </c>
@@ -14083,22 +12366,10 @@
         <v>18</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I141" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J141" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K141" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L141" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
         <v>169</v>
       </c>
@@ -14121,22 +12392,10 @@
         <v>18</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I142" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J142" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K142" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L142" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>170</v>
       </c>
@@ -14159,22 +12418,10 @@
         <v>18</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I143" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J143" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K143" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L143" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>171</v>
       </c>
@@ -14197,22 +12444,10 @@
         <v>20</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I144" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J144" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K144" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L144" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>172</v>
       </c>
@@ -14235,22 +12470,10 @@
         <v>17</v>
       </c>
       <c r="H145" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I145" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J145" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K145" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L145" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>173</v>
       </c>
@@ -14273,22 +12496,10 @@
         <v>18</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I146" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J146" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K146" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L146" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>174</v>
       </c>
@@ -14311,22 +12522,10 @@
         <v>18</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I147" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J147" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K147" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L147" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>175</v>
       </c>
@@ -14349,22 +12548,10 @@
         <v>18</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I148" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J148" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K148" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L148" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>176</v>
       </c>
@@ -14387,22 +12574,10 @@
         <v>18</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I149" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J149" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K149" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L149" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
         <v>177</v>
       </c>
@@ -14425,22 +12600,10 @@
         <v>20</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I150" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J150" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K150" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L150" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>178</v>
       </c>
@@ -14463,22 +12626,10 @@
         <v>17</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I151" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J151" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K151" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L151" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
         <v>179</v>
       </c>
@@ -14501,22 +12652,10 @@
         <v>18</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I152" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J152" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K152" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L152" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
         <v>180</v>
       </c>
@@ -14539,22 +12678,10 @@
         <v>18</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I153" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J153" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K153" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L153" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
         <v>181</v>
       </c>
@@ -14577,22 +12704,10 @@
         <v>18</v>
       </c>
       <c r="H154" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I154" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J154" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K154" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L154" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="13" t="s">
         <v>182</v>
       </c>
@@ -14615,22 +12730,10 @@
         <v>18</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I155" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J155" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K155" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L155" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
         <v>183</v>
       </c>
@@ -14653,22 +12756,10 @@
         <v>20</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I156" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J156" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K156" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L156" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
         <v>184</v>
       </c>
@@ -14691,22 +12782,10 @@
         <v>17</v>
       </c>
       <c r="H157" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I157" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J157" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K157" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L157" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>185</v>
       </c>
@@ -14729,22 +12808,10 @@
         <v>19</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I158" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J158" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K158" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L158" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>186</v>
       </c>
@@ -14767,22 +12834,10 @@
         <v>19</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I159" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J159" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K159" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L159" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
         <v>187</v>
       </c>
@@ -14805,22 +12860,10 @@
         <v>19</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I160" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J160" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K160" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L160" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
         <v>188</v>
       </c>
@@ -14843,22 +12886,10 @@
         <v>19</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I161" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J161" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K161" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L161" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
         <v>189</v>
       </c>
@@ -14881,22 +12912,10 @@
         <v>19</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I162" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J162" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K162" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L162" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
         <v>190</v>
       </c>
@@ -14919,22 +12938,10 @@
         <v>19</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I163" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J163" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K163" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L163" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
         <v>191</v>
       </c>
@@ -14957,22 +12964,10 @@
         <v>19</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I164" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J164" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K164" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L164" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
         <v>192</v>
       </c>
@@ -14995,22 +12990,10 @@
         <v>19</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I165" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J165" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K165" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L165" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
         <v>193</v>
       </c>
@@ -15033,22 +13016,10 @@
         <v>19</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I166" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J166" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K166" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L166" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
         <v>194</v>
       </c>
@@ -15071,22 +13042,10 @@
         <v>19</v>
       </c>
       <c r="H167" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I167" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J167" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K167" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L167" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
         <v>195</v>
       </c>
@@ -15109,22 +13068,10 @@
         <v>19</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I168" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J168" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K168" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L168" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="13" t="s">
         <v>196</v>
       </c>
@@ -15147,22 +13094,10 @@
         <v>19</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I169" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J169" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K169" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L169" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
         <v>197</v>
       </c>
@@ -15185,22 +13120,10 @@
         <v>18</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I170" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J170" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K170" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L170" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
         <v>198</v>
       </c>
@@ -15223,22 +13146,10 @@
         <v>18</v>
       </c>
       <c r="H171" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I171" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J171" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K171" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L171" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>199</v>
       </c>
@@ -15261,22 +13172,10 @@
         <v>18</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I172" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J172" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K172" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L172" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
         <v>200</v>
       </c>
@@ -15299,22 +13198,10 @@
         <v>18</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I173" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J173" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K173" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L173" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
         <v>201</v>
       </c>
@@ -15337,22 +13224,10 @@
         <v>20</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I174" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J174" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K174" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L174" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
         <v>202</v>
       </c>
@@ -15375,22 +13250,10 @@
         <v>17</v>
       </c>
       <c r="H175" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I175" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J175" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K175" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L175" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
         <v>203</v>
       </c>
@@ -15413,22 +13276,10 @@
         <v>18</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I176" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J176" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K176" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L176" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
         <v>204</v>
       </c>
@@ -15451,22 +13302,10 @@
         <v>18</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I177" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J177" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K177" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L177" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
         <v>205</v>
       </c>
@@ -15489,22 +13328,10 @@
         <v>18</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I178" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J178" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K178" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L178" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
         <v>206</v>
       </c>
@@ -15527,22 +13354,10 @@
         <v>18</v>
       </c>
       <c r="H179" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I179" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J179" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K179" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L179" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
         <v>207</v>
       </c>
@@ -15565,22 +13380,10 @@
         <v>20</v>
       </c>
       <c r="H180" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I180" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J180" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K180" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L180" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
         <v>208</v>
       </c>
@@ -15603,19 +13406,7 @@
         <v>17</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I181" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J181" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K181" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="L181" s="3" t="s">
-        <v>285</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change Vww and Vw to be consistent with previous cea assumptions
</commit_message>
<xml_diff>
--- a/cea/databases/CH/Archetypes/Archetypes_properties.xlsx
+++ b/cea/databases/CH/Archetypes/Archetypes_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140" tabRatio="785" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140" tabRatio="785" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -16034,7 +16034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView topLeftCell="A176" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="F206" sqref="F206"/>
     </sheetView>
   </sheetViews>
@@ -23532,7 +23532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -24166,7 +24166,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="13">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -33232,7 +33232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+    <sheetView topLeftCell="A199" workbookViewId="0">
       <selection activeCell="A219" sqref="A219"/>
     </sheetView>
   </sheetViews>

</xml_diff>